<commit_message>
add Log4j2 practices tasks
</commit_message>
<xml_diff>
--- a/resources/EarningsTask.xlsx
+++ b/resources/EarningsTask.xlsx
@@ -2,10 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
@@ -41,6 +43,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -286,6 +289,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -309,7 +313,9 @@
       <c r="B2" s="1">
         <v>400.0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -318,7 +324,9 @@
       <c r="B3" s="1">
         <v>600.0</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -327,7 +335,9 @@
       <c r="B4" s="1">
         <v>200.0</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -336,7 +346,9 @@
       <c r="B5" s="1">
         <v>800.0</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -345,7 +357,9 @@
       <c r="B6" s="1">
         <v>500.0</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="n">
+        <v>3.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>